<commit_message>
fix bugs after changing column order
</commit_message>
<xml_diff>
--- a/TestProject/TestProject/wwwroot/upload/template_2015CSE.xlsx
+++ b/TestProject/TestProject/wwwroot/upload/template_2015CSE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/GraduationAssessment/GraduationAssesment/TestProject/TestProject/wwwroot/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8389D766-0E35-AC4D-AD1F-9CA731D6EEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9F4586-9832-DB40-B244-AC3171E7914F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="165">
   <si>
     <t>입력하려는 졸업기준의 학과(전공)명을 선택하세요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1264,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1281,7 +1281,7 @@
     <col min="7" max="7" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>54</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1314,11 +1314,11 @@
       <c r="D2" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="48">
+    <row r="3" spans="1:8" ht="48">
       <c r="B3" s="4">
         <v>2</v>
       </c>
@@ -1328,11 +1328,11 @@
       <c r="D3" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -1342,11 +1342,11 @@
       <c r="D4" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="B5" s="4">
         <v>4</v>
       </c>
@@ -1356,11 +1356,11 @@
       <c r="D5" s="18">
         <v>2015</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="B6" s="4">
         <v>5</v>
       </c>
@@ -1370,11 +1370,14 @@
       <c r="D6" s="18">
         <v>2015</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1387,17 +1390,20 @@
       <c r="D7" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" t="s">
         <v>92</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>102</v>
       </c>
       <c r="G7" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="B8" s="4">
         <v>7</v>
       </c>
@@ -1407,14 +1413,17 @@
       <c r="D8" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="B9" s="4">
         <v>8</v>
       </c>
@@ -1424,14 +1433,17 @@
       <c r="D9" s="17">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="B10" s="4">
         <v>9</v>
       </c>
@@ -1441,14 +1453,17 @@
       <c r="D10" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="H10" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="B11" s="4">
         <v>10</v>
       </c>
@@ -1458,14 +1473,17 @@
       <c r="D11" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" t="s">
         <v>92</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="B12" s="4">
         <v>11</v>
       </c>
@@ -1475,14 +1493,17 @@
       <c r="D12" s="17">
         <v>4</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="B13" s="4">
         <v>12</v>
       </c>
@@ -1492,14 +1513,17 @@
       <c r="D13" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" t="s">
         <v>92</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="H13" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="B14" s="4">
         <v>13</v>
       </c>
@@ -1509,14 +1533,17 @@
       <c r="D14" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="B15" s="4">
         <v>14</v>
       </c>
@@ -1526,17 +1553,20 @@
       <c r="D15" s="17">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" t="s">
         <v>25</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>103</v>
       </c>
       <c r="G15" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="B16" s="4">
         <v>15</v>
       </c>
@@ -1546,14 +1576,17 @@
       <c r="D16" s="17">
         <v>28</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1566,14 +1599,17 @@
       <c r="D17" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="B18" s="4">
         <v>17</v>
       </c>
@@ -1583,14 +1619,17 @@
       <c r="D18" s="17">
         <v>42</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="H18" s="24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="B19" s="4">
         <v>18</v>
       </c>
@@ -1600,14 +1639,17 @@
       <c r="D19" s="17">
         <v>84</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="B20" s="4">
         <v>19</v>
       </c>
@@ -1617,14 +1659,17 @@
       <c r="D20" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="H20" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="B21" s="4">
         <v>20</v>
       </c>
@@ -1634,14 +1679,17 @@
       <c r="D21" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" t="s">
         <v>95</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="H21" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="B22" s="4">
         <v>21</v>
       </c>
@@ -1651,14 +1699,17 @@
       <c r="D22" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" t="s">
         <v>95</v>
       </c>
-      <c r="F22" s="24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="B23" s="4">
         <v>22</v>
       </c>
@@ -1668,14 +1719,17 @@
       <c r="D23" s="20">
         <v>6</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="H23" s="24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:8">
       <c r="B24" s="4">
         <v>23</v>
       </c>
@@ -1685,14 +1739,17 @@
       <c r="D24" s="20">
         <v>12</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1705,14 +1762,17 @@
       <c r="D25" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F25" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="H25" s="24" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="B26" s="4">
         <v>25</v>
       </c>
@@ -1722,14 +1782,17 @@
       <c r="D26" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" t="s">
         <v>96</v>
       </c>
-      <c r="F26" s="24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="B27" s="4">
         <v>26</v>
       </c>
@@ -1739,17 +1802,20 @@
       <c r="D27" s="20">
         <v>2</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" t="s">
         <v>40</v>
-      </c>
-      <c r="F27" s="24" t="s">
-        <v>103</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="B28" s="4">
         <v>27</v>
       </c>
@@ -1759,15 +1825,18 @@
       <c r="D28" s="20">
         <v>4</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="24" t="s">
-        <v>103</v>
-      </c>
       <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="B29" s="4">
         <v>28</v>
       </c>
@@ -1777,14 +1846,17 @@
       <c r="D29" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" t="s">
         <v>96</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="H29" s="24" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="B30" s="4">
         <v>29</v>
       </c>
@@ -1794,14 +1866,17 @@
       <c r="D30" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="B31" s="4">
         <v>30</v>
       </c>
@@ -1811,17 +1886,20 @@
       <c r="D31" s="20">
         <v>140</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" t="s">
         <v>25</v>
-      </c>
-      <c r="F31" s="24" t="s">
-        <v>103</v>
       </c>
       <c r="G31" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="B32" s="4">
         <v>31</v>
       </c>
@@ -1831,17 +1909,20 @@
       <c r="D32" s="20">
         <v>2</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" t="s">
         <v>27</v>
-      </c>
-      <c r="F32" s="24" t="s">
-        <v>103</v>
       </c>
       <c r="G32" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="48">
+      <c r="H32" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="48">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -1854,14 +1935,17 @@
       <c r="D33" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F33" s="24" t="s">
+      <c r="H33" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="48">
+    <row r="34" spans="1:8" ht="48">
       <c r="B34" s="4">
         <v>33</v>
       </c>
@@ -1871,14 +1955,17 @@
       <c r="D34" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F34" s="24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="B35" s="4">
         <v>34</v>
       </c>
@@ -1888,14 +1975,17 @@
       <c r="D35" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F35" t="s">
         <v>97</v>
       </c>
-      <c r="F35" s="24" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="B36" s="4">
         <v>35</v>
       </c>
@@ -1905,14 +1995,17 @@
       <c r="D36" s="20">
         <v>2</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F36" t="s">
         <v>25</v>
       </c>
-      <c r="F36" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="B37" s="4">
         <v>36</v>
       </c>
@@ -1922,17 +2015,20 @@
       <c r="D37" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" t="s">
         <v>97</v>
-      </c>
-      <c r="F37" s="24" t="s">
-        <v>104</v>
       </c>
       <c r="G37" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="B38" s="4">
         <v>37</v>
       </c>
@@ -1942,14 +2038,17 @@
       <c r="D38" s="20">
         <v>0</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="F38" t="s">
         <v>25</v>
       </c>
-      <c r="F38" s="24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="B39" s="4">
         <v>38</v>
       </c>
@@ -1959,17 +2058,20 @@
       <c r="D39" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="F39" t="s">
         <v>97</v>
-      </c>
-      <c r="F39" s="24" t="s">
-        <v>104</v>
       </c>
       <c r="G39" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="H39" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="B40" s="4">
         <v>39</v>
       </c>
@@ -1979,11 +2081,11 @@
       <c r="D40" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" t="s">
         <v>93</v>
-      </c>
-      <c r="F40" s="24" t="s">
-        <v>102</v>
       </c>
       <c r="G40" t="s">
         <v>47</v>

</xml_diff>